<commit_message>
DP-601: CYC_INTF gererate test script
</commit_message>
<xml_diff>
--- a/src/main/resources/input-excel-file/test-cases/TC_VETC_OPS_CYC_INTF.xlsx
+++ b/src/main/resources/input-excel-file/test-cases/TC_VETC_OPS_CYC_INTF.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutoData\data-etl-reconcilation\src\main\resources\input-excel-file\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code ETL frame work\data-etl-reconcilation\src\main\resources\input-excel-file\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B10681B-D4A1-46A3-B1AE-DC3EE239B57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A2E2A5-DDAC-42EE-A40D-203632B2042C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CYC_INTF" sheetId="4" r:id="rId1"/>
-    <sheet name="LEGEND" sheetId="2" r:id="rId2"/>
+    <sheet name="CYC_INTF_INIT" sheetId="4" r:id="rId1"/>
+    <sheet name=" CYC_INTF_UPDATE_DELETE" sheetId="6" r:id="rId2"/>
+    <sheet name="LEGEND" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CYC_INTF!$A$1:$M$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">' CYC_INTF_UPDATE_DELETE'!$A$1:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CYC_INTF_INIT!$A$1:$M$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="164">
   <si>
     <t>Issue Key</t>
   </si>
@@ -547,9 +549,6 @@
     <t>TargetKeyColumn</t>
   </si>
   <si>
-    <t xml:space="preserve">'CYCLE' AS SRC_STM_CODE </t>
-  </si>
-  <si>
     <t>'CLOSED_CYCLE' AS SRC_STM_NM</t>
   </si>
   <si>
@@ -597,12 +596,137 @@
   <si>
     <t>Target Testing</t>
   </si>
+  <si>
+    <t>UNQ_ID_IN_SRC_STM, EFF_FM_TMS</t>
+  </si>
+  <si>
+    <t>CYC_ANCHOR_ID</t>
+  </si>
+  <si>
+    <t>PPN_TMS</t>
+  </si>
+  <si>
+    <t>CRN_ROW_IND</t>
+  </si>
+  <si>
+    <t>EFF_FM_TMS</t>
+  </si>
+  <si>
+    <t>EFF_TO_TMS</t>
+  </si>
+  <si>
+    <t>Field PCS_DT is less than or equal to current date</t>
+  </si>
+  <si>
+    <t>CURRENT_DATE</t>
+  </si>
+  <si>
+    <t>Field CRN_ROW_IND in (0,1)</t>
+  </si>
+  <si>
+    <t>For records with EFF_TO_TMS = '2400-01-01 23:59:59', field CRN_ROW_IND must be equal to 1</t>
+  </si>
+  <si>
+    <t>EFF_TO_TMS, CRN_ROW_IND</t>
+  </si>
+  <si>
+    <t>[CYC_INTF][EFF_TO_TMS__CRN_ROW_IND]  VerifyValidity</t>
+  </si>
+  <si>
+    <t>At 1 record: EFF_FM_TMS&gt;= EFF_TO_TMS</t>
+  </si>
+  <si>
+    <t>EFF_FM_TMS, EFF_TO_TMS</t>
+  </si>
+  <si>
+    <t>[CYC_INTF][EFF_FM_TMS__EFF_TO_TMS] Check validity</t>
+  </si>
+  <si>
+    <t>EFF_TO_TMS of previous record = EFF_FM_TMS of following record</t>
+  </si>
+  <si>
+    <t>[CYC_INTF][EFF_FM_TMS__EFF_TO_TMS] Check value</t>
+  </si>
+  <si>
+    <t>WITH CYC_INTF_CONVER AS (
+SELECT ROW_NUMBER () OVER (PARTITION BY UNQ_ID_IN_SRC_STM ORDER BY EFF_FM_TMS ASC) AS RANK
+	, UNQ_ID_IN_SRC_STM
+	, EFF_FM_TMS
+	, EFF_TO_TMS
+FROM CYC_INTF
+)
+SELECT a.UNQ_ID_IN_SRC_STM, a.EFF_FM_TMS, a.EFF_TO_TMS, b.EFF_FM_TMS, b.EFF_TO_TMS
+FROM CYC_INTF_CONVER a 
+JOIN CYC_INTF_CONVER b ON a.UNQ_ID_IN_SRC_STM = b.UNQ_ID_IN_SRC_STM AND a.RANK = b.RANK + 1
+WHERE a.EFF_FM_TMS &lt;&gt; b.EFF_TO_TMS</t>
+  </si>
+  <si>
+    <t>CYC_INTF_31</t>
+  </si>
+  <si>
+    <t>CYC_INTF_32</t>
+  </si>
+  <si>
+    <t>CYC_INTF_33</t>
+  </si>
+  <si>
+    <t>CYC_INTF_34</t>
+  </si>
+  <si>
+    <t>CYC_INTF_35</t>
+  </si>
+  <si>
+    <t>CYC_INTF_36</t>
+  </si>
+  <si>
+    <t>CYC_INTF_37</t>
+  </si>
+  <si>
+    <t>'1' AS CRN_ROW_IND</t>
+  </si>
+  <si>
+    <t>CYC_INTF_38</t>
+  </si>
+  <si>
+    <t>Check history record with SCD type 2</t>
+  </si>
+  <si>
+    <t>1. Run Target SQL query
+2. Compare SQL results between source and target table</t>
+  </si>
+  <si>
+    <t>Exits history record with SCD type 2</t>
+  </si>
+  <si>
+    <t>Delete record data</t>
+  </si>
+  <si>
+    <t>1. Prepare test data: delete data record
+2. Run Target SQL query
+3. Compare SQL results between source and target table</t>
+  </si>
+  <si>
+    <t>CYC_INTF_39</t>
+  </si>
+  <si>
+    <t>CYC_INTF_40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Update fields: </t>
+  </si>
+  <si>
+    <t>[CYC_INTF][UNQ_ID_IN_SRC_STM__EFF_FM_TMS]  VerifyUniqueness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'CLOSED_CYCLE' AS SRC_STM_CODE </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -659,14 +783,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -969,7 +1088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1062,18 +1181,27 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1097,7 +1225,78 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1485,1042 +1684,2102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686E8C41-B87D-4004-9D97-3E9D6CC4D6E3}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="80" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="80" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="55.36328125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="83.1796875" style="32" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="32" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="26.36328125" style="32" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="55.36328125" customWidth="1"/>
+    <col min="3" max="3" width="83.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="7" max="7" width="26.36328125" customWidth="1"/>
     <col min="8" max="8" width="27.7265625" style="36" customWidth="1"/>
     <col min="9" max="10" width="22.54296875" style="36" customWidth="1"/>
     <col min="11" max="11" width="54" style="36" customWidth="1"/>
     <col min="12" max="12" width="37.7265625" style="36" customWidth="1"/>
-    <col min="13" max="13" width="26.453125" style="32" customWidth="1"/>
-    <col min="14" max="14" width="18.54296875" style="32" customWidth="1"/>
-    <col min="15" max="16" width="20.81640625" style="32" customWidth="1"/>
-    <col min="17" max="17" width="37.26953125" style="32" customWidth="1"/>
-    <col min="18" max="18" width="12.6328125" style="32" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7265625" style="32" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.81640625" style="32" customWidth="1"/>
-    <col min="21" max="21" width="29.81640625" style="32" customWidth="1"/>
-    <col min="22" max="16384" width="8.7265625" style="32"/>
+    <col min="13" max="13" width="26.453125" customWidth="1"/>
+    <col min="14" max="14" width="18.54296875" customWidth="1"/>
+    <col min="15" max="16" width="20.81640625" customWidth="1"/>
+    <col min="17" max="17" width="37.26953125" customWidth="1"/>
+    <col min="18" max="18" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.81640625" customWidth="1"/>
+    <col min="21" max="21" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="80" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:21" s="39" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="T1" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="str">
+    <row r="2" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="str">
         <f>S2&amp;"_"&amp;ROW()-1</f>
         <v>CYC_INTF_1</v>
       </c>
-      <c r="B2" s="33" t="str">
+      <c r="B2" s="32" t="str">
         <f>"["&amp;S2&amp;"] Verify "&amp;F2</f>
         <v>[CYC_INTF] Verify Metadata</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33" t="s">
+      <c r="C2" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="33" t="str">
+      <c r="K2" s="32" t="str">
         <f>"SELECT * FROM "&amp;O2</f>
         <v>SELECT * FROM CYC_INTF</v>
       </c>
-      <c r="L2" s="33" t="str">
+      <c r="L2" s="32" t="str">
         <f>"DESCRIBE "&amp;R2&amp;"."&amp;S2</f>
         <v>DESCRIBE INTF.CYC_INTF</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="R2" s="33" t="s">
+      <c r="P2" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S2" s="33" t="s">
+      <c r="S2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-    </row>
-    <row r="3" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="str">
-        <f t="shared" ref="A3:A15" si="0">S3&amp;"_"&amp;ROW()-1</f>
+      <c r="T2" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U2" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="str">
+        <f>S3&amp;"_"&amp;ROW()-1</f>
         <v>CYC_INTF_2</v>
       </c>
-      <c r="B3" s="33" t="str">
-        <f>"["&amp;S3&amp;"]["&amp;U3&amp;"]  Verify"&amp;F3</f>
+      <c r="B3" s="32" t="str">
+        <f>"["&amp;O3&amp;"]["&amp;S3&amp;"]  Verify"&amp;F3</f>
+        <v>[CLOSED_CYCLE][CYC_INTF]  VerifyRecord Counts</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="32" t="str">
+        <f>"SELECT COUNT(*)  AS NUM_RECORDS FROM " &amp;N3&amp;"."&amp;O3</f>
+        <v>SELECT COUNT(*)  AS NUM_RECORDS FROM RATING_OWNER.CLOSED_CYCLE</v>
+      </c>
+      <c r="L3" s="32" t="str">
+        <f>"SELECT COUNT(*) AS NUM_RECORDS FROM " &amp;R3&amp;"."&amp;S3</f>
+        <v>SELECT COUNT(*) AS NUM_RECORDS FROM INTF.CYC_INTF</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S3" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U3" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="str">
+        <f t="shared" ref="A4:A31" si="0">S4&amp;"_"&amp;ROW()-1</f>
+        <v>CYC_INTF_3</v>
+      </c>
+      <c r="B4" s="32" t="str">
+        <f>"["&amp;S4&amp;"]["&amp;U4&amp;"]  Verify"&amp;F4</f>
         <v>[CYC_INTF][UNQ_ID_IN_SRC_STM]  VerifyData Values</v>
       </c>
-      <c r="C3" s="33" t="str">
-        <f>"Verify data values between source data:  "&amp;N3&amp;"."&amp;O3&amp;"."&amp;Q3&amp;" and target data: "&amp;R3&amp;"."&amp;S3&amp;"."&amp;U3&amp;" with transformation logic: DIRECT"</f>
+      <c r="C4" s="32" t="str">
+        <f>"Verify data values between source data:  "&amp;N4&amp;"."&amp;O4&amp;"."&amp;Q4&amp;" and target data: "&amp;R4&amp;"."&amp;S4&amp;"."&amp;U4&amp;" with transformation logic: DIRECT"</f>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.CYCLE_ID and target data: INTF.CYC_INTF.UNQ_ID_IN_SRC_STM with transformation logic: DIRECT</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="33" t="s">
+      <c r="F4" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H4" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I4" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J4" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="33" t="str">
-        <f>"SELECT "&amp;Q3&amp;" FROM "&amp;N3&amp;"."&amp;O3&amp;" ORDER BY "&amp;Q3</f>
+      <c r="K4" s="32" t="str">
+        <f>"SELECT "&amp;Q4&amp;" FROM "&amp;N4&amp;"."&amp;O4&amp;" ORDER BY "&amp;Q4</f>
         <v>SELECT CYCLE_ID FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L3" s="33" t="str">
-        <f>"SELECT "&amp;U3&amp;" FROM "&amp;R3&amp;"."&amp;S3&amp;" ORDER BY "&amp;T3</f>
+      <c r="L4" s="32" t="str">
+        <f>"SELECT "&amp;U4&amp;" FROM "&amp;R4&amp;"."&amp;S4&amp;" ORDER BY "&amp;T4</f>
         <v>SELECT UNQ_ID_IN_SRC_STM FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M4" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N4" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="33" t="s">
+      <c r="O4" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P4" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="33" t="s">
+      <c r="Q4" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="R3" s="33" t="s">
+      <c r="R4" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S3" s="33" t="s">
+      <c r="S4" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="33" t="s">
+      <c r="T4" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="U4" s="32" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v>CYC_INTF_3</v>
-      </c>
-      <c r="B4" s="33" t="str">
-        <f t="shared" ref="B4:B9" si="1">"["&amp;S4&amp;"]["&amp;U4&amp;"]  Verify"&amp;F4</f>
-        <v>[CYC_INTF][CYC_CODE]  VerifyData Values</v>
-      </c>
-      <c r="C4" s="33" t="str">
-        <f t="shared" ref="C4:C12" si="2">"Verify data values between source data:  "&amp;N4&amp;"."&amp;O4&amp;"."&amp;Q4&amp;" and target data: "&amp;R4&amp;"."&amp;S4&amp;"."&amp;U4&amp;" with transformation logic: DIRECT"</f>
-        <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.CYCLE_CODE and target data: INTF.CYC_INTF.CYC_CODE with transformation logic: DIRECT</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="33" t="str">
-        <f>"SELECT "&amp;P4&amp;","&amp;Q4&amp;" FROM "&amp;N4&amp;"."&amp;O4&amp;" ORDER BY "&amp;P4</f>
-        <v>SELECT CYCLE_ID,CYCLE_CODE FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
-      </c>
-      <c r="L4" s="33" t="str">
-        <f>"SELECT "&amp;T4&amp;","&amp;U4&amp;" FROM "&amp;R4&amp;"."&amp;S4&amp;" ORDER BY "&amp;T4</f>
-        <v>SELECT UNQ_ID_IN_SRC_STM,CYC_CODE FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
-      </c>
-      <c r="M4" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="N4" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="O4" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="P4" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q4" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="R4" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="S4" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="T4" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="U4" s="33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="str">
+    <row r="5" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="str">
         <f t="shared" si="0"/>
         <v>CYC_INTF_4</v>
       </c>
-      <c r="B5" s="33" t="str">
+      <c r="B5" s="32" t="str">
+        <f t="shared" ref="B5:B10" si="1">"["&amp;S5&amp;"]["&amp;U5&amp;"]  Verify"&amp;F5</f>
+        <v>[CYC_INTF][CYC_CODE]  VerifyData Values</v>
+      </c>
+      <c r="C5" s="32" t="str">
+        <f t="shared" ref="C5:C13" si="2">"Verify data values between source data:  "&amp;N5&amp;"."&amp;O5&amp;"."&amp;Q5&amp;" and target data: "&amp;R5&amp;"."&amp;S5&amp;"."&amp;U5&amp;" with transformation logic: DIRECT"</f>
+        <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.CYCLE_CODE and target data: INTF.CYC_INTF.CYC_CODE with transformation logic: DIRECT</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="32" t="str">
+        <f>"SELECT "&amp;P5&amp;","&amp;Q5&amp;" FROM "&amp;N5&amp;"."&amp;O5&amp;" ORDER BY "&amp;P5</f>
+        <v>SELECT CYCLE_ID,CYCLE_CODE FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
+      </c>
+      <c r="L5" s="32" t="str">
+        <f>"SELECT "&amp;T5&amp;","&amp;U5&amp;" FROM "&amp;R5&amp;"."&amp;S5&amp;" ORDER BY "&amp;T5</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM,CYC_CODE FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="R5" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T5" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U5" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_5</v>
+      </c>
+      <c r="B6" s="32" t="str">
         <f t="shared" si="1"/>
         <v>[CYC_INTF][CYC_NM]  VerifyData Values</v>
       </c>
-      <c r="C5" s="33" t="str">
+      <c r="C6" s="32" t="str">
         <f t="shared" si="2"/>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.CYCLE_NAME and target data: INTF.CYC_INTF.CYC_NM with transformation logic: DIRECT</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="33" t="s">
+      <c r="F6" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H6" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I6" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="J6" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="33" t="str">
-        <f t="shared" ref="K5:K6" si="3">"SELECT "&amp;P5&amp;","&amp;Q5&amp;" FROM "&amp;N5&amp;"."&amp;O5&amp;" ORDER BY "&amp;P5</f>
+      <c r="K6" s="32" t="str">
+        <f t="shared" ref="K6:K7" si="3">"SELECT "&amp;P6&amp;","&amp;Q6&amp;" FROM "&amp;N6&amp;"."&amp;O6&amp;" ORDER BY "&amp;P6</f>
         <v>SELECT CYCLE_ID,CYCLE_NAME FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L5" s="33" t="str">
-        <f t="shared" ref="L5:L12" si="4">"SELECT "&amp;T5&amp;","&amp;U5&amp;" FROM "&amp;R5&amp;"."&amp;S5&amp;" ORDER BY "&amp;T5</f>
+      <c r="L6" s="32" t="str">
+        <f t="shared" ref="L6:L13" si="4">"SELECT "&amp;T6&amp;","&amp;U6&amp;" FROM "&amp;R6&amp;"."&amp;S6&amp;" ORDER BY "&amp;T6</f>
         <v>SELECT UNQ_ID_IN_SRC_STM,CYC_NM FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M6" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N6" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O5" s="33" t="s">
+      <c r="O6" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P5" s="33" t="s">
+      <c r="P6" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q5" s="33" t="s">
+      <c r="Q6" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="R5" s="33" t="s">
+      <c r="R6" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S5" s="33" t="s">
+      <c r="S6" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T5" s="33" t="s">
+      <c r="T6" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U5" s="33" t="s">
+      <c r="U6" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="str">
+    <row r="7" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>CYC_INTF_5</v>
-      </c>
-      <c r="B6" s="33" t="str">
+        <v>CYC_INTF_6</v>
+      </c>
+      <c r="B7" s="32" t="str">
         <f t="shared" si="1"/>
         <v>[CYC_INTF][CYC_STT]  VerifyData Values</v>
       </c>
-      <c r="C6" s="33" t="str">
+      <c r="C7" s="32" t="str">
         <f t="shared" si="2"/>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.STATUS and target data: INTF.CYC_INTF.CYC_STT with transformation logic: DIRECT</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G6" s="33" t="s">
+      <c r="F7" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H7" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I7" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J7" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="33" t="str">
+      <c r="K7" s="32" t="str">
         <f t="shared" si="3"/>
         <v>SELECT CYCLE_ID,STATUS FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L6" s="33" t="str">
+      <c r="L7" s="32" t="str">
         <f t="shared" si="4"/>
         <v>SELECT UNQ_ID_IN_SRC_STM,CYC_STT FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M7" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N7" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="O7" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="P7" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="Q7" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="R6" s="33" t="s">
+      <c r="R7" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S6" s="33" t="s">
+      <c r="S7" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T6" s="33" t="s">
+      <c r="T7" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U6" s="33" t="s">
+      <c r="U7" s="32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="33" t="str">
+    <row r="8" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>CYC_INTF_6</v>
-      </c>
-      <c r="B7" s="33" t="str">
+        <v>CYC_INTF_7</v>
+      </c>
+      <c r="B8" s="32" t="str">
         <f t="shared" si="1"/>
         <v>[CYC_INTF][SRC_STM_CODE]  VerifyData Values</v>
       </c>
-      <c r="C7" s="33" t="str">
+      <c r="C8" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.'CYCLE' AS SRC_STM_CODE  and target data: INTF.CYC_INTF.SRC_STM_CODE with transformation logic: DIRECT</v>
-      </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33" t="s">
+        <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.'CLOSED_CYCLE' AS SRC_STM_CODE  and target data: INTF.CYC_INTF.SRC_STM_CODE with transformation logic: DIRECT</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="33" t="s">
+      <c r="F8" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H8" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I8" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J8" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K7" s="33" t="str">
-        <f t="shared" ref="K7:K12" si="5">"SELECT "&amp;P7&amp;","&amp;Q7&amp;" FROM "&amp;N7&amp;"."&amp;O7&amp;" ORDER BY "&amp;P7</f>
-        <v>SELECT CYCLE_ID,'CYCLE' AS SRC_STM_CODE  FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
-      </c>
-      <c r="L7" s="33" t="str">
+      <c r="K8" s="32" t="str">
+        <f t="shared" ref="K8:K13" si="5">"SELECT "&amp;P8&amp;","&amp;Q8&amp;" FROM "&amp;N8&amp;"."&amp;O8&amp;" ORDER BY "&amp;P8</f>
+        <v>SELECT CYCLE_ID,'CLOSED_CYCLE' AS SRC_STM_CODE  FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
+      </c>
+      <c r="L8" s="32" t="str">
         <f t="shared" si="4"/>
         <v>SELECT UNQ_ID_IN_SRC_STM,SRC_STM_CODE FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M8" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N8" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="O8" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P7" s="33" t="s">
+      <c r="P8" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q7" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="R7" s="33" t="s">
+      <c r="Q8" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="R8" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S7" s="33" t="s">
+      <c r="S8" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T7" s="33" t="s">
+      <c r="T8" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U7" s="33" t="s">
+      <c r="U8" s="32" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="str">
+    <row r="9" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>CYC_INTF_7</v>
-      </c>
-      <c r="B8" s="33" t="str">
+        <v>CYC_INTF_8</v>
+      </c>
+      <c r="B9" s="32" t="str">
         <f t="shared" si="1"/>
         <v>[CYC_INTF][SRC_STM_NM]  VerifyData Values</v>
       </c>
-      <c r="C8" s="33" t="str">
+      <c r="C9" s="32" t="str">
         <f t="shared" si="2"/>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.'CLOSED_CYCLE' AS SRC_STM_NM and target data: INTF.CYC_INTF.SRC_STM_NM with transformation logic: DIRECT</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="33" t="s">
+      <c r="F9" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H9" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I9" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J9" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="33" t="str">
+      <c r="K9" s="32" t="str">
         <f t="shared" si="5"/>
         <v>SELECT CYCLE_ID,'CLOSED_CYCLE' AS SRC_STM_NM FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L8" s="33" t="str">
+      <c r="L9" s="32" t="str">
         <f t="shared" si="4"/>
         <v>SELECT UNQ_ID_IN_SRC_STM,SRC_STM_NM FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M9" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="N9" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O8" s="33" t="s">
+      <c r="O9" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P8" s="33" t="s">
+      <c r="P9" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q8" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="R8" s="33" t="s">
+      <c r="Q9" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="R9" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S8" s="33" t="s">
+      <c r="S9" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T8" s="33" t="s">
+      <c r="T9" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U8" s="33" t="s">
+      <c r="U9" s="32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="str">
+    <row r="10" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>CYC_INTF_8</v>
-      </c>
-      <c r="B9" s="33" t="str">
+        <v>CYC_INTF_9</v>
+      </c>
+      <c r="B10" s="32" t="str">
         <f t="shared" si="1"/>
         <v>[CYC_INTF][PCS_DT]  VerifyData Values</v>
       </c>
-      <c r="C9" s="33" t="str">
+      <c r="C10" s="32" t="str">
         <f t="shared" si="2"/>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.TO_CHAR(to_date(CURRENT_DATE),'yyyy-mm-dd') AS PCS_DT and target data: INTF.CYC_INTF.PCS_DT with transformation logic: DIRECT</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33" t="s">
+      <c r="D10" s="32"/>
+      <c r="E10" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" s="33" t="s">
+      <c r="F10" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H10" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I10" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="J10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K9" s="33" t="str">
+      <c r="K10" s="32" t="str">
         <f t="shared" si="5"/>
         <v>SELECT CYCLE_ID,TO_CHAR(to_date(CURRENT_DATE),'yyyy-mm-dd') AS PCS_DT FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L9" s="33" t="str">
+      <c r="L10" s="32" t="str">
         <f t="shared" si="4"/>
         <v>SELECT UNQ_ID_IN_SRC_STM,PCS_DT FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="M10" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N9" s="33" t="s">
+      <c r="N10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O9" s="33" t="s">
+      <c r="O10" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P9" s="33" t="s">
+      <c r="P10" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q9" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="R9" s="33" t="s">
+      <c r="Q10" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="R10" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S9" s="33" t="s">
+      <c r="S10" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T9" s="33" t="s">
+      <c r="T10" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U9" s="33" t="s">
+      <c r="U10" s="32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="str">
+    <row r="11" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>CYC_INTF_9</v>
-      </c>
-      <c r="B10" s="33" t="str">
-        <f>"["&amp;S10&amp;"][PPN_TMS]  Verify"&amp;F10</f>
+        <v>CYC_INTF_10</v>
+      </c>
+      <c r="B11" s="32" t="str">
+        <f>"["&amp;S11&amp;"][PPN_TMS]  Verify"&amp;F11</f>
         <v>[CYC_INTF][PPN_TMS]  VerifyData Values</v>
       </c>
-      <c r="C10" s="33" t="str">
+      <c r="C11" s="32" t="str">
         <f t="shared" si="2"/>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.REGEXP_SUBSTR(((SYSDATE - TO_DATE('1970-01-01', 'yyyy-MM-dd')) * (24 * 60 * 60 * 1000)),'^[0-9,]{4}') AS PPN_TMS_EXTRACT and target data: INTF.CYC_INTF.SUBSTR(PPN_TMS,0,4) AS PPN_TMS_EXTRACT with transformation logic: DIRECT</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33" t="s">
+      <c r="D11" s="32"/>
+      <c r="E11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" s="33" t="s">
+      <c r="F11" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H11" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I11" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J11" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K10" s="33" t="str">
+      <c r="K11" s="32" t="str">
         <f t="shared" si="5"/>
         <v>SELECT CYCLE_ID,REGEXP_SUBSTR(((SYSDATE - TO_DATE('1970-01-01', 'yyyy-MM-dd')) * (24 * 60 * 60 * 1000)),'^[0-9,]{4}') AS PPN_TMS_EXTRACT FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L10" s="33" t="str">
+      <c r="L11" s="32" t="str">
         <f t="shared" si="4"/>
         <v>SELECT UNQ_ID_IN_SRC_STM,SUBSTR(PPN_TMS,0,4) AS PPN_TMS_EXTRACT FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M11" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N10" s="33" t="s">
+      <c r="N11" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="33" t="s">
+      <c r="O11" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P10" s="33" t="s">
+      <c r="P11" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q10" s="33" t="s">
+      <c r="Q11" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="R11" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S11" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T11" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U11" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="R10" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="S10" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="T10" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="U10" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="34" customFormat="1" ht="126.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="33" t="str">
+    </row>
+    <row r="12" spans="1:21" s="33" customFormat="1" ht="126.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>CYC_INTF_10</v>
-      </c>
-      <c r="B11" s="33" t="str">
-        <f>"["&amp;S11&amp;"]EFF_FM_TMS]  Verify"&amp;F11</f>
+        <v>CYC_INTF_11</v>
+      </c>
+      <c r="B12" s="32" t="str">
+        <f>"["&amp;S12&amp;"]EFF_FM_TMS]  Verify"&amp;F12</f>
         <v>[CYC_INTF]EFF_FM_TMS]  VerifyData Values</v>
       </c>
-      <c r="C11" s="33" t="str">
-        <f>"Verify data values between source data:  "&amp;N11&amp;"."&amp;O11&amp;"."&amp;Q11&amp;" and target data: "&amp;R11&amp;"."&amp;S11&amp;"."&amp;U11&amp;" with transformation logic: DIRECT"</f>
+      <c r="C12" s="32" t="str">
+        <f>"Verify data values between source data:  "&amp;N12&amp;"."&amp;O12&amp;"."&amp;Q12&amp;" and target data: "&amp;R12&amp;"."&amp;S12&amp;"."&amp;U12&amp;" with transformation logic: DIRECT"</f>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.TO_CHAR(CURRENT_DATE,'YYYY-MM-DD') AS EFF_FM_TMS_EXTRACT and target data: INTF.CYC_INTF.SUBSTR(EFF_FM_TMS,0,10) AS EFF_FM_TMS_EXTRACT with transformation logic: DIRECT</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33" t="s">
+      <c r="D12" s="32"/>
+      <c r="E12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="33" t="s">
+      <c r="F12" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H12" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I12" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J11" s="33" t="s">
+      <c r="J12" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="33" t="str">
+      <c r="K12" s="32" t="str">
         <f t="shared" si="5"/>
         <v>SELECT CYCLE_ID,TO_CHAR(CURRENT_DATE,'YYYY-MM-DD') AS EFF_FM_TMS_EXTRACT FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L11" s="33" t="str">
-        <f>"SELECT "&amp;T11&amp;","&amp;U11&amp;" FROM "&amp;R11&amp;"."&amp;S11&amp;" ORDER BY "&amp;T11</f>
+      <c r="L12" s="32" t="str">
+        <f>"SELECT "&amp;T12&amp;","&amp;U12&amp;" FROM "&amp;R12&amp;"."&amp;S12&amp;" ORDER BY "&amp;T12</f>
         <v>SELECT UNQ_ID_IN_SRC_STM,SUBSTR(EFF_FM_TMS,0,10) AS EFF_FM_TMS_EXTRACT FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M12" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N11" s="33" t="s">
+      <c r="N12" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="33" t="s">
+      <c r="O12" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P11" s="33" t="s">
+      <c r="P12" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="R11" s="33" t="s">
+      <c r="Q12" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="R12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S11" s="33" t="s">
+      <c r="S12" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T11" s="33" t="s">
+      <c r="T12" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U11" s="33" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="34" customFormat="1" ht="110" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="str">
+      <c r="U12" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="33" customFormat="1" ht="110" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>CYC_INTF_11</v>
-      </c>
-      <c r="B12" s="33" t="str">
-        <f>"["&amp;S12&amp;"][EFF_TO_TMS]  Verify"&amp;F12</f>
+        <v>CYC_INTF_12</v>
+      </c>
+      <c r="B13" s="32" t="str">
+        <f>"["&amp;S13&amp;"][EFF_TO_TMS]  Verify"&amp;F13</f>
         <v>[CYC_INTF][EFF_TO_TMS]  VerifyData Values</v>
       </c>
-      <c r="C12" s="33" t="str">
+      <c r="C13" s="32" t="str">
         <f t="shared" si="2"/>
         <v>Verify data values between source data:  RATING_OWNER.CLOSED_CYCLE.'2400-01-01' AS EFF_FM_TMS_EXTRACT and target data: INTF.CYC_INTF.SUBSTR(EFF_TO_TMS,0,10) AS EFF_TO_TMS_EXTRACT with transformation logic: DIRECT</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="33" t="s">
+      <c r="F13" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H13" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I13" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="J13" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="33" t="str">
+      <c r="K13" s="32" t="str">
         <f t="shared" si="5"/>
         <v>SELECT CYCLE_ID,'2400-01-01' AS EFF_FM_TMS_EXTRACT FROM RATING_OWNER.CLOSED_CYCLE ORDER BY CYCLE_ID</v>
       </c>
-      <c r="L12" s="33" t="str">
+      <c r="L13" s="32" t="str">
         <f t="shared" si="4"/>
         <v>SELECT UNQ_ID_IN_SRC_STM,SUBSTR(EFF_TO_TMS,0,10) AS EFF_TO_TMS_EXTRACT FROM INTF.CYC_INTF ORDER BY UNQ_ID_IN_SRC_STM</v>
       </c>
-      <c r="M12" s="33" t="s">
+      <c r="M13" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="N13" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O12" s="33" t="s">
+      <c r="O13" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P12" s="33" t="s">
+      <c r="P13" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="Q12" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="R12" s="33" t="s">
+      <c r="Q13" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="R13" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S12" s="33" t="s">
+      <c r="S13" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T12" s="33" t="s">
+      <c r="T13" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="U12" s="33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v>CYC_INTF_12</v>
-      </c>
-      <c r="B13" s="33" t="str">
-        <f>"["&amp;S13&amp;"]["&amp;U13&amp;"]  Verify"&amp;F13</f>
-        <v>[CYC_INTF][UNQ_ID_IN_SRC_STM]  VerifyCompleteness</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="J13" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="L13" s="33" t="str">
-        <f>"SELECT * FROM "&amp;R13&amp;"."&amp;S13&amp;" WHERE "&amp;U13&amp;" is null or "&amp;U13&amp;" =''"&amp;"  or "&amp;U13&amp;" &lt;=0"</f>
-        <v>SELECT * FROM INTF.CYC_INTF WHERE UNQ_ID_IN_SRC_STM is null or UNQ_ID_IN_SRC_STM =''  or UNQ_ID_IN_SRC_STM &lt;=0</v>
-      </c>
-      <c r="M13" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="N13" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="O13" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="P13" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q13" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="R13" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="S13" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="T13" s="33"/>
-      <c r="U13" s="33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="34" customFormat="1" ht="114.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="str">
+      <c r="U13" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="33" customFormat="1" ht="114.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="32" t="str">
         <f t="shared" si="0"/>
         <v>CYC_INTF_13</v>
       </c>
-      <c r="B14" s="33" t="str">
-        <f>"["&amp;S14&amp;"]["&amp;U14&amp;"]  Verify"&amp;F14</f>
-        <v>[CYC_INTF][UNQ_ID_IN_SRC_STM]  VerifyUniqueness</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33" t="s">
+      <c r="B14" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L14" s="32" t="str">
+        <f>"SELECT "&amp;U14&amp;", count(*) as frequency FROM "&amp;R14&amp;"."&amp;S14&amp;" GROUP BY "&amp;U14&amp;" HAVING count(*)&gt;1"</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM, EFF_FM_TMS, count(*) as frequency FROM INTF.CYC_INTF GROUP BY UNQ_ID_IN_SRC_STM, EFF_FM_TMS HAVING count(*)&gt;1</v>
+      </c>
+      <c r="M14" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P14" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q14" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R14" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S14" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="J14" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="K14" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="L14" s="33" t="str">
-        <f>"SELECT "&amp;U14&amp;", count(*) as frequency FROM "&amp;R14&amp;"."&amp;S14&amp;" WHERE "&amp;U14&amp;" is not null or "&amp;U14&amp;" =''"&amp;" or "&amp;U14&amp;" &lt;=0 GROUP BY "&amp;U14&amp;" HAVING count(*)&gt;1"</f>
-        <v>SELECT UNQ_ID_IN_SRC_STM, count(*) as frequency FROM INTF.CYC_INTF WHERE UNQ_ID_IN_SRC_STM is not null or UNQ_ID_IN_SRC_STM ='' or UNQ_ID_IN_SRC_STM &lt;=0 GROUP BY UNQ_ID_IN_SRC_STM HAVING count(*)&gt;1</v>
-      </c>
-      <c r="M14" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="N14" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="O14" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="P14" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q14" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="R14" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="S14" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="T14" s="33"/>
-      <c r="U14" s="33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="34" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="str">
+    </row>
+    <row r="15" spans="1:21" s="33" customFormat="1" ht="114.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="32" t="str">
         <f t="shared" si="0"/>
         <v>CYC_INTF_14</v>
       </c>
-      <c r="B15" s="33" t="str">
-        <f>"["&amp;O15&amp;"]["&amp;S15&amp;"]  Verify"&amp;F15</f>
-        <v>[CLOSED_CYCLE][CYC_INTF]  VerifyRecord Counts</v>
-      </c>
-      <c r="C15" s="33" t="s">
+      <c r="B15" s="32" t="str">
+        <f>"["&amp;S15&amp;"]["&amp;U15&amp;"]  Verify"&amp;F15</f>
+        <v>[CYC_INTF][CYC_ANCHOR_ID]  VerifyUniqueness</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L15" s="32" t="str">
+        <f>"SELECT "&amp;U15&amp;", count(*) as frequency FROM "&amp;R15&amp;"."&amp;S15&amp;" WHERE "&amp;U15&amp;" is not null or "&amp;U15&amp;" =''"&amp;" or "&amp;U15&amp;" &lt;=0 GROUP BY "&amp;U15&amp;" HAVING count(*)&gt;1"</f>
+        <v>SELECT CYC_ANCHOR_ID, count(*) as frequency FROM INTF.CYC_INTF WHERE CYC_ANCHOR_ID is not null or CYC_ANCHOR_ID ='' or CYC_ANCHOR_ID &lt;=0 GROUP BY CYC_ANCHOR_ID HAVING count(*)&gt;1</v>
+      </c>
+      <c r="M15" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="33" t="s">
+      <c r="N15" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O15" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P15" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q15" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R15" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S15" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_15</v>
+      </c>
+      <c r="B16" s="32" t="str">
+        <f>"["&amp;S16&amp;"]["&amp;U16&amp;"]  Verify"&amp;F16</f>
+        <v>[CYC_INTF][UNQ_ID_IN_SRC_STM]  VerifyCompleteness</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I16" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J16" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K15" s="33" t="str">
-        <f>"SELECT COUNT(*)  AS NUM_RECORDS FROM " &amp;N15&amp;"."&amp;O15</f>
-        <v>SELECT COUNT(*)  AS NUM_RECORDS FROM RATING_OWNER.CLOSED_CYCLE</v>
-      </c>
-      <c r="L15" s="33" t="str">
-        <f>"SELECT COUNT(*) AS NUM_RECORDS FROM " &amp;R15&amp;"."&amp;S15</f>
-        <v>SELECT COUNT(*) AS NUM_RECORDS FROM INTF.CYC_INTF</v>
-      </c>
-      <c r="M15" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="N15" s="33" t="s">
+      <c r="K16" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L16" s="32" t="str">
+        <f>"SELECT * FROM "&amp;R16&amp;"."&amp;S16&amp;" WHERE "&amp;U16&amp;" is null or "&amp;U16&amp;" =''"&amp;"  or "&amp;U16&amp;" &lt;=0"</f>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE UNQ_ID_IN_SRC_STM is null or UNQ_ID_IN_SRC_STM =''  or UNQ_ID_IN_SRC_STM &lt;=0</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N16" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="33" t="s">
+      <c r="O16" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P15" s="33" t="s">
+      <c r="P16" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q16" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R16" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S16" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T16" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U16" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_16</v>
+      </c>
+      <c r="B17" s="32" t="str">
+        <f t="shared" ref="B17:B24" si="6">"["&amp;S17&amp;"]["&amp;U17&amp;"]  Verify"&amp;F17</f>
+        <v>[CYC_INTF][PCS_DT]  VerifyCompleteness</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="Q15" s="33" t="s">
+      <c r="H17" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" s="32" t="str">
+        <f>"SELECT * FROM "&amp;R17&amp;"."&amp;S17&amp;" WHERE "&amp;U17&amp;" is null or "&amp;U17&amp;" =''"</f>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE PCS_DT is null or PCS_DT =''</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P17" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q17" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R17" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S17" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T17" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U17" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_17</v>
+      </c>
+      <c r="B18" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>[CYC_INTF][PPN_TMS]  VerifyCompleteness</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="R15" s="33" t="s">
+      <c r="H18" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" s="32" t="str">
+        <f t="shared" ref="L18:L24" si="7">"SELECT * FROM "&amp;R18&amp;"."&amp;S18&amp;" WHERE "&amp;U18&amp;" is null or "&amp;U18&amp;" =''"</f>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE PPN_TMS is null or PPN_TMS =''</v>
+      </c>
+      <c r="M18" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P18" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q18" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R18" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="S15" s="33" t="s">
+      <c r="S18" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
+      <c r="T18" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U18" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_18</v>
+      </c>
+      <c r="B19" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>[CYC_INTF][SRC_STM_CODE]  VerifyCompleteness</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L19" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE SRC_STM_CODE is null or SRC_STM_CODE =''</v>
+      </c>
+      <c r="M19" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N19" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P19" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q19" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R19" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S19" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T19" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U19" s="32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_19</v>
+      </c>
+      <c r="B20" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>[CYC_INTF][SRC_STM_NM]  VerifyCompleteness</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L20" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE SRC_STM_NM is null or SRC_STM_NM =''</v>
+      </c>
+      <c r="M20" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N20" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P20" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q20" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R20" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S20" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T20" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U20" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_20</v>
+      </c>
+      <c r="B21" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>[CYC_INTF][CYC_ANCHOR_ID]  VerifyCompleteness</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L21" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE CYC_ANCHOR_ID is null or CYC_ANCHOR_ID =''</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N21" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O21" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P21" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q21" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R21" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S21" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T21" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U21" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_21</v>
+      </c>
+      <c r="B22" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>[CYC_INTF][CRN_ROW_IND]  VerifyCompleteness</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L22" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE CRN_ROW_IND is null or CRN_ROW_IND =''</v>
+      </c>
+      <c r="M22" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N22" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O22" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P22" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q22" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R22" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S22" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T22" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U22" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_22</v>
+      </c>
+      <c r="B23" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>[CYC_INTF][EFF_FM_TMS]  VerifyCompleteness</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J23" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L23" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE EFF_FM_TMS is null or EFF_FM_TMS =''</v>
+      </c>
+      <c r="M23" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N23" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O23" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P23" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q23" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R23" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S23" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T23" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U23" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_23</v>
+      </c>
+      <c r="B24" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>[CYC_INTF][EFF_TO_TMS]  VerifyCompleteness</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L24" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>SELECT * FROM INTF.CYC_INTF WHERE EFF_TO_TMS is null or EFF_TO_TMS =''</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N24" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O24" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P24" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q24" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R24" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S24" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T24" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="U24" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_24</v>
+      </c>
+      <c r="B25" s="32" t="str">
+        <f t="shared" ref="B25" si="8">"["&amp;S25&amp;"]["&amp;U25&amp;"]  Verify"&amp;F25</f>
+        <v>[CYC_INTF][SRC_STM_CODE]  VerifyValidity</v>
+      </c>
+      <c r="C25" s="32" t="str">
+        <f>"Field "&amp;U25&amp;" only 1 value is '"&amp;Q25&amp;"'"</f>
+        <v>Field SRC_STM_CODE only 1 value is 'CLOSED_CYCLE'</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K25" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L25" s="32" t="str">
+        <f xml:space="preserve"> "SELECT "&amp;T25&amp;", "&amp;U25&amp;" FROM "&amp;S25&amp;" WHERE "&amp;U25&amp;" &lt;&gt; '"&amp;Q25&amp;"'"</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM, SRC_STM_CODE FROM CYC_INTF WHERE SRC_STM_CODE &lt;&gt; 'CLOSED_CYCLE'</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N25" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O25" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P25" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q25" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="R25" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T25" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U25" s="32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_25</v>
+      </c>
+      <c r="B26" s="32" t="str">
+        <f t="shared" ref="B26" si="9">"["&amp;S26&amp;"]["&amp;U26&amp;"]  Verify"&amp;F26</f>
+        <v>[CYC_INTF][SRC_STM_NM]  VerifyValidity</v>
+      </c>
+      <c r="C26" s="32" t="str">
+        <f>"Field "&amp;U26&amp;" only 1 value is '"&amp;Q26&amp;"'"</f>
+        <v>Field SRC_STM_NM only 1 value is 'CLOSED_CYCLE'</v>
+      </c>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L26" s="32" t="str">
+        <f xml:space="preserve"> "SELECT "&amp;T26&amp;", "&amp;U26&amp;" FROM "&amp;S26&amp;" WHERE "&amp;U26&amp;" &lt;&gt; '"&amp;Q26&amp;"'"</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM, SRC_STM_NM FROM CYC_INTF WHERE SRC_STM_NM &lt;&gt; 'CLOSED_CYCLE'</v>
+      </c>
+      <c r="M26" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N26" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O26" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P26" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q26" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="R26" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S26" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T26" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U26" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_26</v>
+      </c>
+      <c r="B27" s="32" t="str">
+        <f t="shared" ref="B27" si="10">"["&amp;S27&amp;"]["&amp;U27&amp;"]  Verify"&amp;F27</f>
+        <v>[CYC_INTF][PCS_DT]  VerifyValidity</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K27" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L27" s="32" t="str">
+        <f xml:space="preserve"> "SELECT "&amp;T27&amp;", "&amp;U27&amp;" FROM "&amp;S27&amp;" WHERE "&amp;U27&amp;" &gt; "&amp;Q27</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM, PCS_DT FROM CYC_INTF WHERE PCS_DT &gt; CURRENT_DATE</v>
+      </c>
+      <c r="M27" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N27" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O27" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P27" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q27" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="R27" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S27" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T27" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U27" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_27</v>
+      </c>
+      <c r="B28" s="32" t="str">
+        <f t="shared" ref="B28" si="11">"["&amp;S28&amp;"]["&amp;U28&amp;"]  Verify"&amp;F28</f>
+        <v>[CYC_INTF][CRN_ROW_IND]  VerifyValidity</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L28" s="32" t="str">
+        <f xml:space="preserve"> "SELECT "&amp;T28&amp;", "&amp;U28&amp;" FROM "&amp;S28&amp;" WHERE "&amp;U28&amp;" NOT IN (0,1)"</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM, CRN_ROW_IND FROM CYC_INTF WHERE CRN_ROW_IND NOT IN (0,1)</v>
+      </c>
+      <c r="M28" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N28" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q28" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R28" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S28" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T28" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U28" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_28</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K29" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L29" s="32" t="str">
+        <f xml:space="preserve"> "SELECT "&amp;T29&amp;", "&amp;U29&amp;" FROM "&amp;S29&amp;" WHERE EFF_TO_TMS = "&amp;"'2400-01-01 23:59:59"&amp;"' AND CRN_ROW_IND &lt;&gt; 1"</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM, EFF_TO_TMS, CRN_ROW_IND FROM CYC_INTF WHERE EFF_TO_TMS = '2400-01-01 23:59:59' AND CRN_ROW_IND &lt;&gt; 1</v>
+      </c>
+      <c r="M29" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N29" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O29" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P29" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q29" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R29" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S29" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T29" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U29" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_29</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K30" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L30" s="32" t="str">
+        <f xml:space="preserve"> "SELECT "&amp;T29&amp;", "&amp;U29&amp;" FROM "&amp;S29&amp;" WHERE EFF_FM_TMS &gt; EFF_TO_TMS"</f>
+        <v>SELECT UNQ_ID_IN_SRC_STM, EFF_TO_TMS, CRN_ROW_IND FROM CYC_INTF WHERE EFF_FM_TMS &gt; EFF_TO_TMS</v>
+      </c>
+      <c r="M30" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N30" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O30" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P30" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q30" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R30" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S30" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T30" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U30" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="33" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>CYC_INTF_30</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L31" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="M31" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O31" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P31" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q31" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R31" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S31" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T31" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U31" s="32" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M15" xr:uid="{686E8C41-B87D-4004-9D97-3E9D6CC4D6E3}"/>
+  <autoFilter ref="A1:M31" xr:uid="{686E8C41-B87D-4004-9D97-3E9D6CC4D6E3}"/>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E15">
+  <conditionalFormatting sqref="E2:E31">
     <cfRule type="cellIs" priority="10" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -2557,7 +3816,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E2:E15</xm:sqref>
+          <xm:sqref>E2:E31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="7" operator="equal" id="{FB95DBF8-C48E-4C75-A5E3-4628BDF84E55}">
@@ -2573,7 +3832,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E2:E15</xm:sqref>
+          <xm:sqref>E2:E31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="1" operator="equal" id="{B6635A36-B7BE-404F-98B2-FF8532399616}">
@@ -2632,7 +3891,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G2:G15</xm:sqref>
+          <xm:sqref>G2:G31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2642,19 +3901,19 @@
           <x14:formula1>
             <xm:f>LEGEND!$A$22:$A$28</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15</xm:sqref>
+          <xm:sqref>F2:F31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F258CDC4-9847-4B22-8B32-E22D3C96DA2B}">
           <x14:formula1>
             <xm:f>LEGEND!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E15</xm:sqref>
+          <xm:sqref>E2:E31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D70D691B-B96C-4821-89E2-C00D09148FE6}">
           <x14:formula1>
             <xm:f>LEGEND!$A$16:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G15</xm:sqref>
+          <xm:sqref>G2:G31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2663,6 +3922,918 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E57DA-B106-4E0E-B438-BB18057F84AC}">
+  <dimension ref="A1:U11"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="46.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="23.36328125" customWidth="1"/>
+    <col min="8" max="8" width="27.7265625" style="36" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" style="36" customWidth="1"/>
+    <col min="10" max="10" width="13" style="36" customWidth="1"/>
+    <col min="11" max="11" width="54" style="36" customWidth="1"/>
+    <col min="12" max="12" width="37.7265625" style="36" customWidth="1"/>
+    <col min="13" max="13" width="26.453125" customWidth="1"/>
+    <col min="14" max="14" width="18.54296875" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="18.36328125" customWidth="1"/>
+    <col min="17" max="17" width="18.453125" customWidth="1"/>
+    <col min="18" max="18" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.81640625" customWidth="1"/>
+    <col min="21" max="21" width="29.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="33" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="32" t="str">
+        <f t="shared" ref="B2:B7" si="0">"["&amp;S2&amp;"]["&amp;U2&amp;"] Update record data"</f>
+        <v>[CYC_INTF][CYC_CODE] Update record data</v>
+      </c>
+      <c r="C2" s="32" t="str">
+        <f>"Update data record, field "&amp;U2</f>
+        <v>Update data record, field CYC_CODE</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="32" t="str">
+        <f t="shared" ref="K2:K9" si="1">"SELECT "&amp;P2&amp;", "&amp;Q2&amp;" FROM "&amp;O2&amp;" WHERE "&amp;P2&amp;" IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) "</f>
+        <v xml:space="preserve">SELECT CYCLE_ID, CYCLE_CODE FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L2" s="32" t="str">
+        <f t="shared" ref="L2:L9" si="2">"Select UNQ_ID_IN_SRC_STM, "&amp;U2&amp;" From "&amp;S2&amp;" where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'"</f>
+        <v>Select UNQ_ID_IN_SRC_STM, CYC_CODE From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U2" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>[CYC_INTF][CYC_NM] Update record data</v>
+      </c>
+      <c r="C3" s="32" t="str">
+        <f t="shared" ref="C3:C9" si="3">"Update data record, field "&amp;U3</f>
+        <v>Update data record, field CYC_NM</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SELECT CYCLE_ID, CYCLE_NAME FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L3" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v>Select UNQ_ID_IN_SRC_STM, CYC_NM From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S3" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U3" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>[CYC_INTF][CYC_STT] Update record data</v>
+      </c>
+      <c r="C4" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>Update data record, field CYC_STT</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SELECT CYCLE_ID, STATUS FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L4" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v>Select UNQ_ID_IN_SRC_STM, CYC_STT From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="R4" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S4" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U4" s="32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>[CYC_INTF][PCS_DT] Update record data</v>
+      </c>
+      <c r="C5" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>Update data record, field PCS_DT</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SELECT CYCLE_ID, TO_CHAR(to_date(CURRENT_DATE),'yyyy-mm-dd') AS PCS_DT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L5" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v>Select UNQ_ID_IN_SRC_STM, PCS_DT From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="R5" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T5" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U5" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="32" t="str">
+        <f t="shared" ref="B6" si="4">"["&amp;S6&amp;"]["&amp;U6&amp;"] Update record data"</f>
+        <v>[CYC_INTF][SUBSTR(PPN_TMS,0,4) AS PPN_TMS_EXTRACT] Update record data</v>
+      </c>
+      <c r="C6" s="32" t="str">
+        <f t="shared" ref="C6" si="5">"Update data record, field "&amp;U6</f>
+        <v>Update data record, field SUBSTR(PPN_TMS,0,4) AS PPN_TMS_EXTRACT</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SELECT CYCLE_ID, REGEXP_SUBSTR(((SYSDATE - TO_DATE('1970-01-01', 'yyyy-MM-dd')) * (24 * 60 * 60 * 1000)),'^[0-9,]{4}') AS PPN_TMS_EXTRACT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L6" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v>Select UNQ_ID_IN_SRC_STM, SUBSTR(PPN_TMS,0,4) AS PPN_TMS_EXTRACT From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N6" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P6" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q6" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="R6" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S6" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T6" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U6" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>[CYC_INTF][CRN_ROW_IND] Update record data</v>
+      </c>
+      <c r="C7" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>Update data record, field CRN_ROW_IND</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SELECT CYCLE_ID, '1' AS CRN_ROW_IND FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L7" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v>Select UNQ_ID_IN_SRC_STM, CRN_ROW_IND From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P7" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q7" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="R7" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T7" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U7" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="32" t="str">
+        <f>"["&amp;S8&amp;"]["&amp;U8&amp;"] Update record data"</f>
+        <v>[CYC_INTF][SUBSTR(EFF_FM_TMS,0,10) AS EFF_FM_TMS_EXTRACT] Update record data</v>
+      </c>
+      <c r="C8" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>Update data record, field SUBSTR(EFF_FM_TMS,0,10) AS EFF_FM_TMS_EXTRACT</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SELECT CYCLE_ID, TO_CHAR(CURRENT_DATE,'YYYY-MM-DD') AS EFF_FM_TMS_EXTRACT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L8" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v>Select UNQ_ID_IN_SRC_STM, SUBSTR(EFF_FM_TMS,0,10) AS EFF_FM_TMS_EXTRACT From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P8" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q8" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="R8" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S8" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T8" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U8" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="32" t="str">
+        <f t="shared" ref="B9" si="6">"["&amp;S9&amp;"]["&amp;U9&amp;"] Update record data"</f>
+        <v>[CYC_INTF][SUBSTR(EFF_TO_TMS,0,10) AS EFF_TO_TMS_EXTRACT] Update record data</v>
+      </c>
+      <c r="C9" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>Update data record, field SUBSTR(EFF_TO_TMS,0,10) AS EFF_TO_TMS_EXTRACT</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">SELECT CYCLE_ID, '2400-01-01' AS EFF_FM_TMS_EXTRACT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+      </c>
+      <c r="L9" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v>Select UNQ_ID_IN_SRC_STM, SUBSTR(EFF_TO_TMS,0,10) AS EFF_TO_TMS_EXTRACT From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q9" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="R9" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S9" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T9" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U9" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="33" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="32" t="str">
+        <f>"["&amp;S10&amp;"][Update record data] Check history record"</f>
+        <v>[CYC_INTF][Update record data] Check history record</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="32" t="str">
+        <f>"Select * From "&amp;S10&amp;" where UNQ_ID_IN_SRC_STM IN (9599, 4107, 1004, 1014) AND eff_to_tms &lt;&gt; '2400-01-01 23:59:59'"</f>
+        <v>Select * From CYC_INTF where UNQ_ID_IN_SRC_STM IN (9599, 4107, 1004, 1014) AND eff_to_tms &lt;&gt; '2400-01-01 23:59:59'</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P10" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q10" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="R10" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S10" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T10" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U10" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="33" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A11" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="32" t="str">
+        <f>"["&amp;S11&amp;"] Delete record data"</f>
+        <v>[CYC_INTF] Delete record data</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" s="32" t="str">
+        <f>"Select * From "&amp;S11&amp;" where UNQ_ID_IN_SRC_STM IN (1247, 5126)"</f>
+        <v>Select * From CYC_INTF where UNQ_ID_IN_SRC_STM IN (1247, 5126)</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P11" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q11" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="R11" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="S11" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="T11" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U11" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:M2" xr:uid="{686E8C41-B87D-4004-9D97-3E9D6CC4D6E3}"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="E2:E11">
+    <cfRule type="cellIs" priority="10" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{4FDCB8C6-26FC-478B-91C2-EA4A379154A5}">
+            <xm:f>LEGEND!$A$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C5700"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{1BAD32E4-132F-4D52-BB9B-DFC8FF44DA2E}">
+            <xm:f>LEGEND!$A$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E2:E11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{B5B95749-956E-49F0-8BC9-5D6E291695A2}">
+            <xm:f>LEGEND!$A$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E2:E11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{1C7F129A-6D42-42BE-B32F-340134946555}">
+            <xm:f>LEGEND!$A$18</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF99CC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{7E9A12BA-3EE8-493F-8267-1AB0F1D7E215}">
+            <xm:f>LEGEND!$A$18</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF66CC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{EFFC6E51-F314-4253-B30D-531F8F612580}">
+            <xm:f>LEGEND!$A$18</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{71341F3B-3208-421E-B1B8-33262DF66AE2}">
+            <xm:f>LEGEND!$A$17</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{788AF0F7-CCFC-40E1-A05D-938068AF2D63}">
+            <xm:f>LEGEND!$A$16</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G2:G11</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5217386-E36D-46E4-B092-912EDB6B89D3}">
+          <x14:formula1>
+            <xm:f>LEGEND!$A$16:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7FA21508-14B2-4A0D-A791-109FA85E3F80}">
+          <x14:formula1>
+            <xm:f>LEGEND!$A$4:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{73904994-D6E9-46A4-8CAF-E9B8D4EBA002}">
+          <x14:formula1>
+            <xm:f>LEGEND!$A$22:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7083CF65-FCB6-4458-B691-8DF886E4EA77}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
@@ -2705,10 +4876,10 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2919,10 +5090,10 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="42"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -3069,10 +5240,10 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="42"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3164,7 +5335,7 @@
     </row>
     <row r="17" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>23</v>
@@ -3255,11 +5426,11 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -3354,7 +5525,7 @@
     </row>
     <row r="23" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>30</v>
@@ -3394,7 +5565,7 @@
         <v>32</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3428,7 +5599,7 @@
         <v>34</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3462,7 +5633,7 @@
         <v>36</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -3496,7 +5667,7 @@
         <v>37</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -3641,11 +5812,11 @@
       <c r="Z31" s="28"/>
     </row>
     <row r="32" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="42"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>

</xml_diff>

<commit_message>
DP-601: CYC_INTF gererate test scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/input-excel-file/test-cases/TC_VETC_OPS_CYC_INTF.xlsx
+++ b/src/main/resources/input-excel-file/test-cases/TC_VETC_OPS_CYC_INTF.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code ETL frame work\data-etl-reconcilation\src\main\resources\input-excel-file\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A2E2A5-DDAC-42EE-A40D-203632B2042C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6E40F-D451-4916-933B-EC878651A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CYC_INTF_INIT" sheetId="4" r:id="rId1"/>
-    <sheet name=" CYC_INTF_UPDATE_DELETE" sheetId="6" r:id="rId2"/>
+    <sheet name="CYC_INTF_UPDATE_DELETE" sheetId="6" r:id="rId2"/>
     <sheet name="LEGEND" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">' CYC_INTF_UPDATE_DELETE'!$A$1:$M$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CYC_INTF_INIT!$A$1:$M$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CYC_INTF_UPDATE_DELETE!$A$1:$M$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1686,11 +1686,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686E8C41-B87D-4004-9D97-3E9D6CC4D6E3}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="80" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3925,7 +3925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533E57DA-B106-4E0E-B438-BB18057F84AC}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="K2" s="32" t="str">
         <f t="shared" ref="K2:K9" si="1">"SELECT "&amp;P2&amp;", "&amp;Q2&amp;" FROM "&amp;O2&amp;" WHERE "&amp;P2&amp;" IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) "</f>
-        <v xml:space="preserve">SELECT CYCLE_ID, CYCLE_CODE FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, CYCLE_CODE FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L2" s="32" t="str">
         <f t="shared" ref="L2:L9" si="2">"Select UNQ_ID_IN_SRC_STM, "&amp;U2&amp;" From "&amp;S2&amp;" where UNQ_ID_IN_SRC_STM IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) AND eff_to_tms = '2400-01-01 23:59:59'"</f>
@@ -4068,7 +4068,7 @@
         <v>83</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P2" s="32" t="s">
         <v>96</v>
@@ -4122,7 +4122,7 @@
       </c>
       <c r="K3" s="32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SELECT CYCLE_ID, CYCLE_NAME FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, CYCLE_NAME FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L3" s="32" t="str">
         <f t="shared" si="2"/>
@@ -4135,7 +4135,7 @@
         <v>83</v>
       </c>
       <c r="O3" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P3" s="32" t="s">
         <v>96</v>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="K4" s="32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SELECT CYCLE_ID, STATUS FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, STATUS FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L4" s="32" t="str">
         <f t="shared" si="2"/>
@@ -4202,7 +4202,7 @@
         <v>83</v>
       </c>
       <c r="O4" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P4" s="32" t="s">
         <v>96</v>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="K5" s="32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SELECT CYCLE_ID, TO_CHAR(to_date(CURRENT_DATE),'yyyy-mm-dd') AS PCS_DT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, TO_CHAR(to_date(CURRENT_DATE),'yyyy-mm-dd') AS PCS_DT FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L5" s="32" t="str">
         <f t="shared" si="2"/>
@@ -4269,7 +4269,7 @@
         <v>83</v>
       </c>
       <c r="O5" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P5" s="32" t="s">
         <v>96</v>
@@ -4295,11 +4295,11 @@
         <v>149</v>
       </c>
       <c r="B6" s="32" t="str">
-        <f t="shared" ref="B6" si="4">"["&amp;S6&amp;"]["&amp;U6&amp;"] Update record data"</f>
-        <v>[CYC_INTF][SUBSTR(PPN_TMS,0,4) AS PPN_TMS_EXTRACT] Update record data</v>
+        <f>"["&amp;S6&amp;"][PPN_TMS] Update record data"</f>
+        <v>[CYC_INTF][PPN_TMS] Update record data</v>
       </c>
       <c r="C6" s="32" t="str">
-        <f t="shared" ref="C6" si="5">"Update data record, field "&amp;U6</f>
+        <f t="shared" ref="C6" si="4">"Update data record, field "&amp;U6</f>
         <v>Update data record, field SUBSTR(PPN_TMS,0,4) AS PPN_TMS_EXTRACT</v>
       </c>
       <c r="D6" s="34"/>
@@ -4323,7 +4323,7 @@
       </c>
       <c r="K6" s="32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SELECT CYCLE_ID, REGEXP_SUBSTR(((SYSDATE - TO_DATE('1970-01-01', 'yyyy-MM-dd')) * (24 * 60 * 60 * 1000)),'^[0-9,]{4}') AS PPN_TMS_EXTRACT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, REGEXP_SUBSTR(((SYSDATE - TO_DATE('1970-01-01', 'yyyy-MM-dd')) * (24 * 60 * 60 * 1000)),'^[0-9,]{4}') AS PPN_TMS_EXTRACT FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L6" s="32" t="str">
         <f t="shared" si="2"/>
@@ -4336,7 +4336,7 @@
         <v>83</v>
       </c>
       <c r="O6" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P6" s="32" t="s">
         <v>96</v>
@@ -4390,7 +4390,7 @@
       </c>
       <c r="K7" s="32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SELECT CYCLE_ID, '1' AS CRN_ROW_IND FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, '1' AS CRN_ROW_IND FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L7" s="32" t="str">
         <f t="shared" si="2"/>
@@ -4403,7 +4403,7 @@
         <v>83</v>
       </c>
       <c r="O7" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P7" s="32" t="s">
         <v>96</v>
@@ -4429,8 +4429,8 @@
         <v>151</v>
       </c>
       <c r="B8" s="32" t="str">
-        <f>"["&amp;S8&amp;"]["&amp;U8&amp;"] Update record data"</f>
-        <v>[CYC_INTF][SUBSTR(EFF_FM_TMS,0,10) AS EFF_FM_TMS_EXTRACT] Update record data</v>
+        <f>"["&amp;S8&amp;"][EFF_FM_TMS] Update record data"</f>
+        <v>[CYC_INTF][EFF_FM_TMS] Update record data</v>
       </c>
       <c r="C8" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="K8" s="32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SELECT CYCLE_ID, TO_CHAR(CURRENT_DATE,'YYYY-MM-DD') AS EFF_FM_TMS_EXTRACT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, TO_CHAR(CURRENT_DATE,'YYYY-MM-DD') AS EFF_FM_TMS_EXTRACT FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L8" s="32" t="str">
         <f t="shared" si="2"/>
@@ -4470,7 +4470,7 @@
         <v>83</v>
       </c>
       <c r="O8" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P8" s="32" t="s">
         <v>96</v>
@@ -4496,8 +4496,8 @@
         <v>153</v>
       </c>
       <c r="B9" s="32" t="str">
-        <f t="shared" ref="B9" si="6">"["&amp;S9&amp;"]["&amp;U9&amp;"] Update record data"</f>
-        <v>[CYC_INTF][SUBSTR(EFF_TO_TMS,0,10) AS EFF_TO_TMS_EXTRACT] Update record data</v>
+        <f>"["&amp;S9&amp;"][EFF_TO_TMS] Update record data"</f>
+        <v>[CYC_INTF][EFF_TO_TMS] Update record data</v>
       </c>
       <c r="C9" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="K9" s="32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SELECT CYCLE_ID, '2400-01-01' AS EFF_FM_TMS_EXTRACT FROM CYC_INTF WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
+        <v xml:space="preserve">SELECT CYCLE_ID, '2400-01-01' AS EFF_FM_TMS_EXTRACT FROM CLOSED_CYCLE WHERE CYCLE_ID IN (9599, 1004, 1014, 2275, 3551, 1247, 5126, 4107, 6774) </v>
       </c>
       <c r="L9" s="32" t="str">
         <f t="shared" si="2"/>
@@ -4537,7 +4537,7 @@
         <v>83</v>
       </c>
       <c r="O9" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P9" s="32" t="s">
         <v>96</v>
@@ -4602,7 +4602,7 @@
         <v>83</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P10" s="32" t="s">
         <v>96</v>
@@ -4667,7 +4667,7 @@
         <v>83</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P11" s="32" t="s">
         <v>96</v>

</xml_diff>